<commit_message>
All features added Code documented Ready for testing
</commit_message>
<xml_diff>
--- a/DDTuneTrack/bin/Debug/DDRentalTunes2015.xlsx
+++ b/DDTuneTrack/bin/Debug/DDRentalTunes2015.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="30">
   <si>
     <t>Tune Type</t>
   </si>
@@ -33,40 +33,79 @@
     <t>Staff</t>
   </si>
   <si>
+    <t>Notes</t>
+  </si>
+  <si>
     <t>Accident Calibration</t>
   </si>
   <si>
     <t>DM</t>
   </si>
   <si>
+    <t>Regular Tune Test</t>
+  </si>
+  <si>
     <t>Wax Only</t>
   </si>
   <si>
     <t>RG</t>
   </si>
   <si>
-    <t>457r578</t>
+    <t>Midnight Test 3</t>
+  </si>
+  <si>
+    <t>Will it do the thing?</t>
+  </si>
+  <si>
+    <t>after thing</t>
+  </si>
+  <si>
+    <t>TB</t>
   </si>
   <si>
     <t>Performance Tune</t>
   </si>
   <si>
-    <t>boken</t>
-  </si>
-  <si>
-    <t>TB</t>
-  </si>
-  <si>
-    <t>toe strap, 326</t>
-  </si>
-  <si>
-    <t>toe strap</t>
-  </si>
-  <si>
-    <t>Top sheet epoxy</t>
-  </si>
-  <si>
-    <t>so broked</t>
+    <t>New the thing</t>
+  </si>
+  <si>
+    <t>not blank</t>
+  </si>
+  <si>
+    <t>after blank</t>
+  </si>
+  <si>
+    <t>45678ikjhewsdfg</t>
+  </si>
+  <si>
+    <t>Not a blank note</t>
+  </si>
+  <si>
+    <t>blank note</t>
+  </si>
+  <si>
+    <t>not a blank note 1</t>
+  </si>
+  <si>
+    <t>Not a blank note 2</t>
+  </si>
+  <si>
+    <t>not blank 1</t>
+  </si>
+  <si>
+    <t>blank 1</t>
+  </si>
+  <si>
+    <t>not blank 2</t>
+  </si>
+  <si>
+    <t>Not blank 1</t>
+  </si>
+  <si>
+    <t>Blank 1</t>
+  </si>
+  <si>
+    <t>Not blank 2</t>
   </si>
 </sst>
 </file>
@@ -415,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="A2" sqref="A2:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,230 +484,567 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>23536</v>
+        <v>123456</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2">
-        <v>42166</v>
+        <v>42288</v>
       </c>
       <c r="D2" s="2">
-        <v>42166</v>
+        <v>42288</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>34678</v>
+        <v>12345</v>
       </c>
       <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2">
+        <v>42288</v>
+      </c>
+      <c r="D3" s="2">
+        <v>42288</v>
+      </c>
+      <c r="E3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2">
-        <v>42166</v>
-      </c>
-      <c r="D3" s="2">
-        <v>42166</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4">
+        <v>12345</v>
+      </c>
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
       <c r="C4" s="2">
-        <v>42166</v>
+        <v>42288</v>
       </c>
       <c r="D4" s="2">
-        <v>42166</v>
+        <v>42288</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>457679</v>
+        <v>12345</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="2">
-        <v>42166</v>
+        <v>42288</v>
       </c>
       <c r="D5" s="2">
-        <v>42166</v>
+        <v>42288</v>
       </c>
       <c r="E5" t="s">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c r="F5">
+        <v>34567</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>80</v>
+        <v>2345678</v>
       </c>
       <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="2">
+        <v>42288</v>
+      </c>
+      <c r="D6" s="2">
+        <v>42288</v>
+      </c>
+      <c r="E6" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="2">
-        <v>42166</v>
-      </c>
-      <c r="D6" s="2">
-        <v>42166</v>
-      </c>
-      <c r="E6" t="s">
-        <v>8</v>
+      <c r="F6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>12355</v>
+        <v>2345678</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C7" s="2">
-        <v>42258</v>
+        <v>42288</v>
       </c>
       <c r="D7" s="2">
-        <v>42258</v>
+        <v>42288</v>
       </c>
       <c r="E7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7">
-        <v>234</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>12345</v>
+        <v>876543</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C8" s="2">
-        <v>42258</v>
+        <v>42288</v>
       </c>
       <c r="D8" s="2">
-        <v>42258</v>
+        <v>42288</v>
       </c>
       <c r="E8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>132556</v>
+        <v>1234567</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C9" s="2">
-        <v>42258</v>
+        <v>42288</v>
       </c>
       <c r="D9" s="2">
-        <v>42258</v>
+        <v>42288</v>
       </c>
       <c r="E9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="F9">
+        <v>5678</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>124</v>
+        <v>12345678</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C10" s="2">
-        <v>42258</v>
+        <v>42288</v>
       </c>
       <c r="D10" s="2">
-        <v>42258</v>
+        <v>42288</v>
       </c>
       <c r="E10" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="F10" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>1345</v>
+        <v>1234567</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C11" s="2">
-        <v>42258</v>
+        <v>42288</v>
       </c>
       <c r="D11" s="2">
-        <v>42258</v>
+        <v>42288</v>
       </c>
       <c r="E11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F11" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>134</v>
+        <v>87654</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C12" s="2">
-        <v>42258</v>
+        <v>42288</v>
       </c>
       <c r="D12" s="2">
-        <v>42258</v>
+        <v>42288</v>
       </c>
       <c r="E12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12">
-        <v>245</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>2345</v>
+        <v>765325</v>
       </c>
       <c r="B13" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C13" s="2">
-        <v>42258</v>
+        <v>42288</v>
       </c>
       <c r="D13" s="2">
-        <v>42258</v>
+        <v>42288</v>
       </c>
       <c r="E13" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F13" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>87654</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="2">
+        <v>42288</v>
+      </c>
+      <c r="D14" s="2">
+        <v>42288</v>
+      </c>
+      <c r="E14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14">
+        <v>876545678</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>678987654</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="2">
+        <v>42288</v>
+      </c>
+      <c r="D15" s="2">
+        <v>42288</v>
+      </c>
+      <c r="E15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>567898765</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="2">
+        <v>42288</v>
+      </c>
+      <c r="D16" s="2">
+        <v>42288</v>
+      </c>
+      <c r="E16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="2">
+        <v>42288</v>
+      </c>
+      <c r="D17" s="2">
+        <v>42288</v>
+      </c>
+      <c r="E17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>565432345</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="2">
+        <v>42288</v>
+      </c>
+      <c r="D18" s="2">
+        <v>42288</v>
+      </c>
+      <c r="E18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>34567876</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="2">
+        <v>42288</v>
+      </c>
+      <c r="D19" s="2">
+        <v>42288</v>
+      </c>
+      <c r="E19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1234567</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="2">
+        <v>42288</v>
+      </c>
+      <c r="D20" s="2">
+        <v>42288</v>
+      </c>
+      <c r="E20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>76543</v>
+      </c>
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="2">
+        <v>42288</v>
+      </c>
+      <c r="D21" s="2">
+        <v>42288</v>
+      </c>
+      <c r="E21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="2">
+        <v>42288</v>
+      </c>
+      <c r="D22" s="2">
+        <v>42288</v>
+      </c>
+      <c r="E22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="2">
+        <v>42288</v>
+      </c>
+      <c r="D23" s="2">
+        <v>42288</v>
+      </c>
+      <c r="E23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="2">
+        <v>42288</v>
+      </c>
+      <c r="D24" s="2">
+        <v>42288</v>
+      </c>
+      <c r="E24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="2">
+        <v>42288</v>
+      </c>
+      <c r="D25" s="2">
+        <v>42288</v>
+      </c>
+      <c r="E25" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" s="2">
+        <v>42288</v>
+      </c>
+      <c r="D26" s="2">
+        <v>42288</v>
+      </c>
+      <c r="E26" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" s="2">
+        <v>42288</v>
+      </c>
+      <c r="D27" s="2">
+        <v>42288</v>
+      </c>
+      <c r="E27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="2">
+        <v>42288</v>
+      </c>
+      <c r="D28" s="2">
+        <v>42288</v>
+      </c>
+      <c r="E28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="2">
+        <v>42288</v>
+      </c>
+      <c r="D29" s="2">
+        <v>42288</v>
+      </c>
+      <c r="E29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" s="2">
+        <v>42288</v>
+      </c>
+      <c r="D30" s="2">
+        <v>42288</v>
+      </c>
+      <c r="E30" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Increased timer tick value to 1 hour Fixed a bug where validation labels weren't hidden on selecting a tune list item. Removed unnecessary numRows attribute from TuneList Add icon file and test cases file.
</commit_message>
<xml_diff>
--- a/DDTuneTrack/bin/Debug/DDRentalTunes2015.xlsx
+++ b/DDTuneTrack/bin/Debug/DDRentalTunes2015.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="31">
   <si>
     <t>Tune Type</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>Not blank 2</t>
+  </si>
+  <si>
+    <t>4567890-</t>
   </si>
 </sst>
 </file>
@@ -454,7 +457,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:F3"/>
@@ -1045,6 +1048,103 @@
       </c>
       <c r="F30" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>9876543</v>
+      </c>
+      <c r="B31" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" s="2">
+        <v>42288</v>
+      </c>
+      <c r="D31" s="2">
+        <v>42288</v>
+      </c>
+      <c r="E31" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31">
+        <v>7654326</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>7654</v>
+      </c>
+      <c r="B32" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" s="2">
+        <v>42288</v>
+      </c>
+      <c r="D32" s="2">
+        <v>42288</v>
+      </c>
+      <c r="E32" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>456789</v>
+      </c>
+      <c r="B33" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" s="2">
+        <v>42045</v>
+      </c>
+      <c r="D33" s="2">
+        <v>42288</v>
+      </c>
+      <c r="E33" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33">
+        <v>9876543</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>4567890</v>
+      </c>
+      <c r="B34" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" s="2">
+        <v>42015</v>
+      </c>
+      <c r="D34" s="2">
+        <v>42015</v>
+      </c>
+      <c r="E34" t="s">
+        <v>7</v>
+      </c>
+      <c r="F34">
+        <v>98765</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>30</v>
+      </c>
+      <c r="B35" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" s="2">
+        <v>42401</v>
+      </c>
+      <c r="D35" s="2">
+        <v>42401</v>
+      </c>
+      <c r="E35" t="s">
+        <v>10</v>
+      </c>
+      <c r="F35">
+        <v>567890</v>
       </c>
     </row>
   </sheetData>

</xml_diff>